<commit_message>
changed photographs after review
</commit_message>
<xml_diff>
--- a/R-Scripts/covariants_test.xlsx
+++ b/R-Scripts/covariants_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\Geometric Morphometrics\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\R-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9CDAD6-2FFE-4AB4-8C1E-08D8027FAFA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E70652-90A5-4293-9D2E-1A8A17D60504}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="750" windowWidth="12330" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="13680" yWindow="705" windowWidth="12330" windowHeight="14190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="69">
   <si>
     <t>acotar_gelina_ech_g.JPG</t>
   </si>
@@ -173,6 +173,72 @@
   </si>
   <si>
     <t>AEOROLET</t>
+  </si>
+  <si>
+    <t>apopra_gelina_mesgab_g.JPG</t>
+  </si>
+  <si>
+    <t>apshir_gelina_mesagr_g.JPG</t>
+  </si>
+  <si>
+    <t>artfor_gelina_messph_g.JPG</t>
+  </si>
+  <si>
+    <t>atetsi_gelina_mesate_g.JPG</t>
+  </si>
+  <si>
+    <t>bicver_gelina_meslym_g.JPG</t>
+  </si>
+  <si>
+    <t>coeful_gelina_mescoe_g.JPG</t>
+  </si>
+  <si>
+    <t>crespi_gelina_mescer_g.JPG</t>
+  </si>
+  <si>
+    <t>cryban_gelina_mesmes_g.JPG</t>
+  </si>
+  <si>
+    <t>dicsp_gelina_mesglo_g.JPG</t>
+  </si>
+  <si>
+    <t>melsp_gelina_mesmel_g.JPG</t>
+  </si>
+  <si>
+    <t>necsp_gelina_mesgor_g.JPG</t>
+  </si>
+  <si>
+    <t>odospi_gelina_mesisc_g.JPG</t>
+  </si>
+  <si>
+    <t>parsap_gelina_mesbar_g.JPG</t>
+  </si>
+  <si>
+    <t>picmel_gelina_mesnem_g.JPG</t>
+  </si>
+  <si>
+    <t>steaxi_gelina_mesvag_g.JPG</t>
+  </si>
+  <si>
+    <t>steins_gelina_mesnem_g.JPG</t>
+  </si>
+  <si>
+    <t>Gelini</t>
+  </si>
+  <si>
+    <t>Gel</t>
+  </si>
+  <si>
+    <t>Mes</t>
+  </si>
+  <si>
+    <t>Ech</t>
+  </si>
+  <si>
+    <t>Mesostini</t>
+  </si>
+  <si>
+    <t>Echthrini</t>
   </si>
 </sst>
 </file>
@@ -524,10 +590,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +604,7 @@
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -552,12 +618,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="str">
-        <f t="shared" ref="B2:B31" si="0" xml:space="preserve"> IF(ISNUMBER(SEARCH("ECH",A2)), "Echthrini", "Gelini")</f>
+        <f t="shared" ref="B2:B31" si="0" xml:space="preserve"> IF(ISNUMBER(SEARCH("ech",A2)), "Echthrini", IF(ISNUMBER(SEARCH("mes",A2)), "Mestioni", "Gelini"))</f>
         <v>Echthrini</v>
       </c>
       <c r="C2" t="str">
@@ -569,7 +635,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -581,11 +647,11 @@
         <v>37</v>
       </c>
       <c r="D3" t="str">
-        <f t="shared" ref="D3:D31" si="1" xml:space="preserve"> IF(ISNUMBER(SEARCH("_O",A3)), "OPEN", "CLOSED")</f>
+        <f t="shared" ref="D3:D47" si="1" xml:space="preserve"> IF(ISNUMBER(SEARCH("_O",A3)), "OPEN", "CLOSED")</f>
         <v>OPEN</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -601,7 +667,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -617,7 +683,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -634,7 +700,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -651,7 +717,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -667,8 +733,14 @@
         <f t="shared" si="1"/>
         <v>CLOSED</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -684,8 +756,14 @@
         <f t="shared" si="1"/>
         <v>CLOSED</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -700,8 +778,14 @@
         <f t="shared" si="1"/>
         <v>OPEN</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -717,7 +801,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -733,7 +817,7 @@
         <v>OPEN</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -749,7 +833,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -766,7 +850,7 @@
         <v>CLOSED</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -782,7 +866,7 @@
         <v>OPEN</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1045,6 +1129,214 @@
       <c r="D31" t="str">
         <f t="shared" si="1"/>
         <v>OPEN</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" t="str">
+        <f xml:space="preserve"> IF(ISNUMBER(SEARCH("ech",A32)), "Echthrini", IF(ISNUMBER(SEARCH("mes",A32)), "Mestioni", "Gelini"))</f>
+        <v>Mestioni</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" t="str">
+        <f t="shared" ref="B33:B47" si="3" xml:space="preserve"> IF(ISNUMBER(SEARCH("ech",A33)), "Echthrini", IF(ISNUMBER(SEARCH("mes",A33)), "Mestioni", "Gelini"))</f>
+        <v>Mestioni</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>50</v>
+      </c>
+      <c r="B35" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>51</v>
+      </c>
+      <c r="B36" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>52</v>
+      </c>
+      <c r="B37" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>53</v>
+      </c>
+      <c r="B38" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>55</v>
+      </c>
+      <c r="B40" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>56</v>
+      </c>
+      <c r="B41" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>57</v>
+      </c>
+      <c r="B42" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>58</v>
+      </c>
+      <c r="B43" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>61</v>
+      </c>
+      <c r="B46" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" t="str">
+        <f t="shared" si="3"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="D47" t="str">
+        <f t="shared" si="1"/>
+        <v>CLOSED</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed images so that new functions work, added 3d plot
</commit_message>
<xml_diff>
--- a/R-Scripts/covariants_test.xlsx
+++ b/R-Scripts/covariants_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robin\Dropbox\Mein PC (Gemeinsamer-PC)\Documents\GitHub\Ichneumonidae\R-Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E883E1CB-813E-47E7-A506-EDE2E6C21FC6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E02D9B88-8AE4-4297-A5ED-4AF92D3259F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="100">
   <si>
     <t>acotar_gelina_g_echech.JPG</t>
   </si>
@@ -51,9 +51,6 @@
     <t>echrel_gelina_g_echech.JPG</t>
   </si>
   <si>
-    <t>javsp_gelina_g_echech.JPG</t>
-  </si>
-  <si>
     <t>litnoh_gelina_g_echech.JPG</t>
   </si>
   <si>
@@ -69,9 +66,6 @@
     <t>parple_gelina_g_echech.JPG</t>
   </si>
   <si>
-    <t>plasp_gelina_g_echech.JPG</t>
-  </si>
-  <si>
     <t>pledig_gelina_g_echech.JPG</t>
   </si>
   <si>
@@ -147,15 +141,6 @@
     <t>cryban_gelina_g_mesmes.JPG</t>
   </si>
   <si>
-    <t>dicsp_gelina_g_mesglo.JPG</t>
-  </si>
-  <si>
-    <t>melsp_gelina_g_mesmel.JPG</t>
-  </si>
-  <si>
-    <t>necsp_gelina_g_mesgor.JPG</t>
-  </si>
-  <si>
     <t>odospi_gelina_g_mesisc.JPG</t>
   </si>
   <si>
@@ -171,9 +156,6 @@
     <t>steins_gelina_g_mesnem.JPG</t>
   </si>
   <si>
-    <t>astmet_gelina_o_gelchi.JPG</t>
-  </si>
-  <si>
     <t>fossil_gelina_g_gelina.JPG</t>
   </si>
   <si>
@@ -270,31 +252,88 @@
     <t>schgra_gelina_g_echech.JPG</t>
   </si>
   <si>
+    <t>uchmar_gelina_g_gelphy.JPG</t>
+  </si>
+  <si>
+    <t>amypul_gelina_g_gelmas.JPG</t>
+  </si>
+  <si>
+    <t>apotru_gelina_o_gelmas.JPG</t>
+  </si>
+  <si>
+    <t>chithy_gelina_o_gelchi.JPG</t>
+  </si>
+  <si>
+    <t>diapro_gelina_g_gelacr.JPG</t>
+  </si>
+  <si>
+    <t>endsub_gelina_g_gelend.JPG</t>
+  </si>
+  <si>
+    <t>eudsp._gelina_o_gelacr.JPG</t>
+  </si>
+  <si>
+    <t>gabdes_gelina_o_gelchi.JPG</t>
+  </si>
+  <si>
+    <t>gnoten_gelina_g_gelphy.JPG</t>
+  </si>
+  <si>
+    <t>hembip_gelina_g_gelhem.JPG</t>
+  </si>
+  <si>
+    <t>isdlyc_gelina_o_gelacr.JPG</t>
+  </si>
+  <si>
+    <t>liesp._gelina_o_gelchi.JPG</t>
+  </si>
+  <si>
+    <t>odoacu_gelina_o_gelchi.JPG</t>
+  </si>
+  <si>
+    <t>parafas_gelina_o_gelchi.JPG</t>
+  </si>
+  <si>
+    <t>retsp._gelina_g_gelbat.JPG</t>
+  </si>
+  <si>
+    <t>stidec_gelina_o_gelmas.JPG</t>
+  </si>
+  <si>
+    <t>teldec_gelina_g_gelmas.JPG</t>
+  </si>
+  <si>
+    <t>TRIBE</t>
+  </si>
+  <si>
+    <t>AREOLET</t>
+  </si>
+  <si>
+    <t>SUBTRIBE</t>
+  </si>
+  <si>
     <t xml:space="preserve">ID </t>
   </si>
   <si>
-    <t>TRIBE</t>
-  </si>
-  <si>
-    <t>AREOLET</t>
-  </si>
-  <si>
-    <t>SUBTRIBE</t>
-  </si>
-  <si>
-    <t>fossil</t>
-  </si>
-  <si>
     <t>rhequa_gelina_g_geleth.JPG</t>
   </si>
   <si>
-    <t>CREATOR</t>
-  </si>
-  <si>
-    <t>ROBIN</t>
-  </si>
-  <si>
-    <t>OLIVIA</t>
+    <t>FOSSIL</t>
+  </si>
+  <si>
+    <t>javsp._gelina_g_echech.JPG</t>
+  </si>
+  <si>
+    <t>plasp._gelina_g_echech.JPG</t>
+  </si>
+  <si>
+    <t>dicsp._gelina_g_mesglo.JPG</t>
+  </si>
+  <si>
+    <t>melsp._gelina_g_mesmel.JPG</t>
+  </si>
+  <si>
+    <t>necsp._gelina_g_mesgor.JPG</t>
   </si>
 </sst>
 </file>
@@ -318,12 +357,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -338,9 +383,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -366,7 +412,7 @@
       <sheetName val="Subtribes"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="1">
           <cell r="B1" t="str">
@@ -926,35 +972,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E80"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I69" sqref="I69"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>79</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>80</v>
+        <v>90</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -970,11 +1010,8 @@
         <f>VLOOKUP(LEFT(RIGHT(A2,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -990,11 +1027,8 @@
         <f>VLOOKUP(LEFT(RIGHT(A3,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1010,11 +1044,8 @@
         <f>VLOOKUP(LEFT(RIGHT(A4,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E4" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1030,11 +1061,8 @@
         <f>VLOOKUP(LEFT(RIGHT(A5,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E5" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1050,33 +1078,27 @@
         <f>VLOOKUP(LEFT(RIGHT(A6,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="str">
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B7" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Echthrini</v>
       </c>
-      <c r="C7" t="str">
-        <f t="shared" si="3"/>
-        <v>CLOSED</v>
-      </c>
-      <c r="D7" t="str">
+      <c r="C7" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D7" s="2" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A7,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="str">
         <f t="shared" si="2"/>
@@ -1090,13 +1112,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A8,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="str">
         <f t="shared" si="2"/>
@@ -1110,13 +1129,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A9,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="str">
         <f t="shared" si="2"/>
@@ -1130,13 +1146,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A10,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E10" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="str">
         <f t="shared" si="2"/>
@@ -1150,13 +1163,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A11,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="str">
         <f t="shared" si="2"/>
@@ -1170,33 +1180,27 @@
         <f>VLOOKUP(LEFT(RIGHT(A12,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" t="str">
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B13" s="2" t="str">
         <f t="shared" si="2"/>
         <v>Echthrini</v>
       </c>
-      <c r="C13" t="str">
-        <f t="shared" si="3"/>
-        <v>CLOSED</v>
-      </c>
-      <c r="D13" t="str">
+      <c r="C13" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D13" s="2" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A13,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E13" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B14" t="str">
         <f t="shared" si="2"/>
@@ -1210,13 +1214,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A14,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="str">
         <f t="shared" si="2"/>
@@ -1230,13 +1231,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A15,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E15" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B16" t="str">
         <f t="shared" si="2"/>
@@ -1250,13 +1248,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A16,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E16" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B17" t="str">
         <f t="shared" si="2"/>
@@ -1270,13 +1265,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A17,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>gnypetomorphina</v>
       </c>
-      <c r="E17" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B18" t="str">
         <f t="shared" si="2"/>
@@ -1290,13 +1282,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A18,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>mastrina</v>
       </c>
-      <c r="E18" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B19" t="str">
         <f t="shared" si="2"/>
@@ -1310,13 +1299,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A19,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>acrolytina</v>
       </c>
-      <c r="E19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B20" t="str">
         <f t="shared" si="2"/>
@@ -1330,13 +1316,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A20,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>chiroticina</v>
       </c>
-      <c r="E20" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B21" t="str">
         <f t="shared" si="2"/>
@@ -1350,13 +1333,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A21,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>gelina</v>
       </c>
-      <c r="E21" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B22" t="str">
         <f t="shared" si="2"/>
@@ -1370,13 +1350,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A22,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>endaseina</v>
       </c>
-      <c r="E22" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B23" t="str">
         <f t="shared" si="2"/>
@@ -1390,13 +1367,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A23,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>rothneyiina</v>
       </c>
-      <c r="E23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B24" t="str">
         <f t="shared" si="2"/>
@@ -1410,13 +1384,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A24,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>chiroticina</v>
       </c>
-      <c r="E24" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" t="str">
         <f t="shared" si="2"/>
@@ -1430,13 +1401,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A25,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>phygadeuontina</v>
       </c>
-      <c r="E25" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B26" t="str">
         <f t="shared" si="2"/>
@@ -1450,13 +1418,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A26,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>hemitelina</v>
       </c>
-      <c r="E26" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B27" t="str">
         <f t="shared" si="2"/>
@@ -1470,13 +1435,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A27,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>bathytrichina</v>
       </c>
-      <c r="E27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="B28" t="str">
         <f t="shared" si="2"/>
@@ -1490,13 +1452,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A28,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>ethelurgina</v>
       </c>
-      <c r="E28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B29" t="str">
         <f t="shared" si="2"/>
@@ -1510,13 +1469,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A29,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>stilpnina</v>
       </c>
-      <c r="E29" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" t="str">
         <f t="shared" si="2"/>
@@ -1530,13 +1486,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A30,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>acrolytina</v>
       </c>
-      <c r="E30" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B31" t="str">
         <f t="shared" si="2"/>
@@ -1550,13 +1503,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A31,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>cremnodina</v>
       </c>
-      <c r="E31" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B32" t="str">
         <f t="shared" si="2"/>
@@ -1570,13 +1520,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A32,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>gabuniina</v>
       </c>
-      <c r="E32" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B33" t="str">
         <f t="shared" si="2"/>
@@ -1590,13 +1537,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A33,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>agrothereutina</v>
       </c>
-      <c r="E33" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B34" t="str">
         <f t="shared" si="2"/>
@@ -1610,13 +1554,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A34,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>sphecophagina</v>
       </c>
-      <c r="E34" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B35" t="str">
         <f t="shared" si="2"/>
@@ -1630,13 +1571,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A35,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>ateleute</v>
       </c>
-      <c r="E35" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B36" t="str">
         <f t="shared" si="2"/>
@@ -1650,13 +1588,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A36,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>lymeonina</v>
       </c>
-      <c r="E36" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B37" t="str">
         <f t="shared" si="2"/>
@@ -1670,13 +1605,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A37,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>coesula</v>
       </c>
-      <c r="E37" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B38" t="str">
         <f t="shared" si="2"/>
@@ -1690,13 +1622,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A38,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>ceratocryptina</v>
       </c>
-      <c r="E38" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B39" t="str">
         <f t="shared" si="2"/>
@@ -1710,73 +1639,61 @@
         <f>VLOOKUP(LEFT(RIGHT(A39,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>mesostenina</v>
       </c>
-      <c r="E39" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>37</v>
-      </c>
-      <c r="B40" t="str">
-        <f t="shared" si="2"/>
-        <v>Mestioni</v>
-      </c>
-      <c r="C40" t="str">
-        <f t="shared" si="3"/>
-        <v>CLOSED</v>
-      </c>
-      <c r="D40" t="str">
+    </row>
+    <row r="40" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B40" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="C40" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D40" s="2" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A40,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>glodianina</v>
       </c>
-      <c r="E40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>38</v>
-      </c>
-      <c r="B41" t="str">
-        <f t="shared" si="2"/>
-        <v>Mestioni</v>
-      </c>
-      <c r="C41" t="str">
-        <f t="shared" si="3"/>
-        <v>CLOSED</v>
-      </c>
-      <c r="D41" t="str">
+    </row>
+    <row r="41" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B41" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="C41" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D41" s="2" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A41,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>melanocryptus</v>
       </c>
-      <c r="E41" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>39</v>
-      </c>
-      <c r="B42" t="str">
-        <f t="shared" si="2"/>
-        <v>Mestioni</v>
-      </c>
-      <c r="C42" t="str">
-        <f t="shared" si="3"/>
-        <v>CLOSED</v>
-      </c>
-      <c r="D42" t="str">
+    </row>
+    <row r="42" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B42" s="2" t="str">
+        <f t="shared" si="2"/>
+        <v>Mestioni</v>
+      </c>
+      <c r="C42" s="2" t="str">
+        <f t="shared" si="3"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D42" s="2" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A42,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>goryphina</v>
       </c>
-      <c r="E42" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B43" t="str">
         <f t="shared" si="2"/>
@@ -1790,13 +1707,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A43,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>ischnina</v>
       </c>
-      <c r="E43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B44" t="str">
         <f t="shared" si="2"/>
@@ -1810,13 +1724,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A44,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>baryceratina</v>
       </c>
-      <c r="E44" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B45" t="str">
         <f t="shared" si="2"/>
@@ -1830,13 +1741,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A45,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>nematopodiina</v>
       </c>
-      <c r="E45" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B46" t="str">
         <f t="shared" si="2"/>
@@ -1850,13 +1758,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A46,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>vagenathina</v>
       </c>
-      <c r="E46" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="B47" t="str">
         <f t="shared" si="2"/>
@@ -1870,13 +1775,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A47,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>nematopodiina</v>
       </c>
-      <c r="E47" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B48" t="str">
         <f t="shared" si="2"/>
@@ -1884,41 +1786,36 @@
       </c>
       <c r="C48" t="str">
         <f t="shared" si="3"/>
-        <v>OPEN</v>
-      </c>
-      <c r="D48" t="str">
-        <f>VLOOKUP(LEFT(RIGHT(A48,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>chiroticina</v>
-      </c>
-      <c r="E48" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+        <v>CLOSED</v>
+      </c>
+      <c r="D48" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" t="s">
-        <v>82</v>
+        <v>41</v>
+      </c>
+      <c r="B49" t="str">
+        <f t="shared" si="2"/>
+        <v>Mestioni</v>
       </c>
       <c r="C49" t="str">
         <f t="shared" si="3"/>
         <v>CLOSED</v>
       </c>
-      <c r="D49" t="s">
-        <v>82</v>
-      </c>
-      <c r="E49" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D49" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A49,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="B50" t="str">
         <f t="shared" si="2"/>
-        <v>Mestioni</v>
+        <v>Echthrini</v>
       </c>
       <c r="C50" t="str">
         <f t="shared" si="3"/>
@@ -1926,19 +1823,16 @@
       </c>
       <c r="D50" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A50,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E50" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+        <v>echthrini</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B51" t="str">
         <f t="shared" si="2"/>
-        <v>Echthrini</v>
+        <v>Mestioni</v>
       </c>
       <c r="C51" t="str">
         <f t="shared" si="3"/>
@@ -1946,15 +1840,12 @@
       </c>
       <c r="D51" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A51,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>echthrini</v>
-      </c>
-      <c r="E51" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+        <v>agrothereutina</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="B52" t="str">
         <f t="shared" si="2"/>
@@ -1968,13 +1859,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A52,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>agrothereutina</v>
       </c>
-      <c r="E52" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B53" t="str">
         <f t="shared" si="2"/>
@@ -1982,19 +1870,16 @@
       </c>
       <c r="C53" t="str">
         <f t="shared" si="3"/>
-        <v>CLOSED</v>
+        <v>OPEN</v>
       </c>
       <c r="D53" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A53,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>agrothereutina</v>
-      </c>
-      <c r="E53" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+        <v>baryceratina</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="B54" t="str">
         <f t="shared" si="2"/>
@@ -2002,19 +1887,16 @@
       </c>
       <c r="C54" t="str">
         <f t="shared" si="3"/>
-        <v>OPEN</v>
+        <v>CLOSED</v>
       </c>
       <c r="D54" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A54,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>baryceratina</v>
-      </c>
-      <c r="E54" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B55" t="str">
         <f t="shared" si="2"/>
@@ -2026,15 +1908,12 @@
       </c>
       <c r="D55" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A55,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E55" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+        <v>baryceratina</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B56" t="str">
         <f t="shared" si="2"/>
@@ -2048,13 +1927,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A56,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>baryceratina</v>
       </c>
-      <c r="E56" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B57" t="str">
         <f t="shared" si="2"/>
@@ -2068,13 +1944,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A57,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>baryceratina</v>
       </c>
-      <c r="E57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B58" t="str">
         <f t="shared" si="2"/>
@@ -2088,13 +1961,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A58,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>baryceratina</v>
       </c>
-      <c r="E58" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="B59" t="str">
         <f t="shared" si="2"/>
@@ -2106,15 +1976,12 @@
       </c>
       <c r="D59" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A59,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>baryceratina</v>
-      </c>
-      <c r="E59" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B60" t="str">
         <f t="shared" si="2"/>
@@ -2128,13 +1995,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A60,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>ischnina</v>
       </c>
-      <c r="E60" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="B61" t="str">
         <f t="shared" si="2"/>
@@ -2146,15 +2010,12 @@
       </c>
       <c r="D61" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A61,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E61" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+        <v>agrothereutina</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B62" t="str">
         <f t="shared" si="2"/>
@@ -2168,13 +2029,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A62,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>agrothereutina</v>
       </c>
-      <c r="E62" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B63" t="str">
         <f t="shared" si="2"/>
@@ -2188,13 +2046,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A63,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>agrothereutina</v>
       </c>
-      <c r="E63" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B64" t="str">
         <f t="shared" si="2"/>
@@ -2206,15 +2061,12 @@
       </c>
       <c r="D64" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A64,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>agrothereutina</v>
-      </c>
-      <c r="E64" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B65" t="str">
         <f t="shared" si="2"/>
@@ -2222,19 +2074,16 @@
       </c>
       <c r="C65" t="str">
         <f t="shared" si="3"/>
-        <v>CLOSED</v>
+        <v>OPEN</v>
       </c>
       <c r="D65" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A65,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E65" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+        <v>baryceratina</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B66" t="str">
         <f t="shared" si="2"/>
@@ -2242,39 +2091,33 @@
       </c>
       <c r="C66" t="str">
         <f t="shared" si="3"/>
-        <v>OPEN</v>
+        <v>CLOSED</v>
       </c>
       <c r="D66" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A66,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>baryceratina</v>
-      </c>
-      <c r="E66" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B80" si="4" xml:space="preserve"> IF(ISNUMBER(SEARCH("ech",A67)), "Echthrini", IF(ISNUMBER(SEARCH("mes",A67)), "Mestioni", "Gelini"))</f>
+        <f t="shared" ref="B67:B96" si="4" xml:space="preserve"> IF(ISNUMBER(SEARCH("ech",A67)), "Echthrini", IF(ISNUMBER(SEARCH("mes",A67)), "Mestioni", "Gelini"))</f>
         <v>Mestioni</v>
       </c>
       <c r="C67" t="str">
-        <f t="shared" ref="C67:C80" si="5" xml:space="preserve"> IF(ISNUMBER(SEARCH("_o",A67)), "OPEN", "CLOSED")</f>
+        <f t="shared" ref="C67:C96" si="5" xml:space="preserve"> IF(ISNUMBER(SEARCH("_o",A67)), "OPEN", "CLOSED")</f>
         <v>CLOSED</v>
       </c>
       <c r="D67" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A67,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E67" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+        <v>agrothereutina</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B68" t="str">
         <f t="shared" si="4"/>
@@ -2286,15 +2129,12 @@
       </c>
       <c r="D68" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A68,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>agrothereutina</v>
-      </c>
-      <c r="E68" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+        <v>ischnina</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="B69" t="str">
         <f t="shared" si="4"/>
@@ -2306,15 +2146,12 @@
       </c>
       <c r="D69" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A69,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>ischnina</v>
-      </c>
-      <c r="E69" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+        <v>agrothereutina</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B70" t="str">
         <f t="shared" si="4"/>
@@ -2326,19 +2163,16 @@
       </c>
       <c r="D70" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A70,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>agrothereutina</v>
-      </c>
-      <c r="E70" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+        <v>baryceratina</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B71" t="str">
         <f t="shared" si="4"/>
-        <v>Mestioni</v>
+        <v>Echthrini</v>
       </c>
       <c r="C71" t="str">
         <f t="shared" si="5"/>
@@ -2346,15 +2180,12 @@
       </c>
       <c r="D71" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A71,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>baryceratina</v>
-      </c>
-      <c r="E71" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+        <v>echthrini</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B72" t="str">
         <f t="shared" si="4"/>
@@ -2368,13 +2199,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A72,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E72" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B73" t="str">
         <f t="shared" si="4"/>
@@ -2382,19 +2210,16 @@
       </c>
       <c r="C73" t="str">
         <f t="shared" si="5"/>
-        <v>CLOSED</v>
+        <v>OPEN</v>
       </c>
       <c r="D73" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A73,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E73" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="B74" t="str">
         <f t="shared" si="4"/>
@@ -2402,19 +2227,16 @@
       </c>
       <c r="C74" t="str">
         <f t="shared" si="5"/>
-        <v>OPEN</v>
+        <v>CLOSED</v>
       </c>
       <c r="D74" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A74,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E74" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B75" t="str">
         <f t="shared" si="4"/>
@@ -2428,13 +2250,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A75,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E75" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="B76" t="str">
         <f t="shared" si="4"/>
@@ -2448,13 +2267,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A76,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E76" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B77" t="str">
         <f t="shared" si="4"/>
@@ -2468,13 +2284,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A77,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E77" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B78" t="str">
         <f t="shared" si="4"/>
@@ -2488,13 +2301,10 @@
         <f>VLOOKUP(LEFT(RIGHT(A78,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E78" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B79" t="str">
         <f t="shared" si="4"/>
@@ -2508,17 +2318,14 @@
         <f>VLOOKUP(LEFT(RIGHT(A79,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
         <v>echthrini</v>
       </c>
-      <c r="E79" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B80" t="str">
         <f t="shared" si="4"/>
-        <v>Echthrini</v>
+        <v>Gelini</v>
       </c>
       <c r="C80" t="str">
         <f t="shared" si="5"/>
@@ -2526,10 +2333,279 @@
       </c>
       <c r="D80" t="str">
         <f>VLOOKUP(LEFT(RIGHT(A80,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
-        <v>echthrini</v>
-      </c>
-      <c r="E80" t="s">
+        <v>phygadeuontina</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>73</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D81" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A81,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>mastrina</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>74</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D82" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A82,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>mastrina</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>75</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D83" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A83,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>chiroticina</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>76</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D84" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A84,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>acrolytina</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>77</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D85" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A85,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>endaseina</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>78</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D86" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A86,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>acrolytina</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D87" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A87,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>chiroticina</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>80</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D88" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A88,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>phygadeuontina</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>81</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D89" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A89,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>hemitelina</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D90" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A90,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>acrolytina</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>83</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D91" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A91,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>chiroticina</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D92" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A92,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>chiroticina</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
         <v>85</v>
+      </c>
+      <c r="B93" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D93" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A93,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>chiroticina</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>86</v>
+      </c>
+      <c r="B94" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D94" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A94,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>bathytrichina</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>87</v>
+      </c>
+      <c r="B95" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" si="5"/>
+        <v>OPEN</v>
+      </c>
+      <c r="D95" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A95,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>mastrina</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>88</v>
+      </c>
+      <c r="B96" t="str">
+        <f t="shared" si="4"/>
+        <v>Gelini</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" si="5"/>
+        <v>CLOSED</v>
+      </c>
+      <c r="D96" t="str">
+        <f>VLOOKUP(LEFT(RIGHT(A96,7), 3), [1]Subtribes!$A$1:$B$35, 2, FALSE)</f>
+        <v>mastrina</v>
       </c>
     </row>
   </sheetData>

</xml_diff>